<commit_message>
update part 2 code and excel
</commit_message>
<xml_diff>
--- a/Homework2/images/Excel Histo Data Graphs.xlsx
+++ b/Homework2/images/Excel Histo Data Graphs.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>CHI</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Uniform Int</t>
-  </si>
-  <si>
-    <t>Discreet</t>
   </si>
   <si>
     <t>Cauchy</t>
@@ -43861,7 +43858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AH18" sqref="AH18:AH19"/>
     </sheetView>
   </sheetViews>
@@ -47813,7 +47810,7 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47829,13 +47826,13 @@
         <v>33</v>
       </c>
       <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
-      </c>
-      <c r="P1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>